<commit_message>
Finished 3 files of 43 files+
</commit_message>
<xml_diff>
--- a/output/CodeSystem-cs-thcc-43filetype.xlsx
+++ b/output/CodeSystem-cs-thcc-43filetype.xlsx
@@ -24,7 +24,7 @@
     <t>URL</t>
   </si>
   <si>
-    <t>http://terms.sil-th.org/Codesystem/cs-thcc-43filetype</t>
+    <t>https://terms.sil-th.org/Codesystem/cs-thcc-43file-type</t>
   </si>
   <si>
     <t>Version</t>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2022-07-31T02:30:06+07:00</t>
+    <t>2022-07-31T15:19:09+07:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>